<commit_message>
MAJ Google Analytics 4
</commit_message>
<xml_diff>
--- a/Modèle-audit-SEO.xlsx
+++ b/Modèle-audit-SEO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Sauvegarde de Mes cours\Projet 4\Projet\Starting website 2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2788342E-261A-401F-9392-B39A4C3AAE87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1330C03F-C993-4E15-B767-ACD1534078AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2318" yWindow="630" windowWidth="25612" windowHeight="14040" tabRatio="149" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2993" yWindow="1305" windowWidth="25612" windowHeight="14040" tabRatio="149" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -1175,6 +1175,692 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">Des balises </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>&lt;meta&gt;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> importantes sont absentes</t>
+    </r>
+  </si>
+  <si>
+    <t>Ne pas oublier ces balises</t>
+  </si>
+  <si>
+    <t>Ajouter ces balises</t>
+  </si>
+  <si>
+    <t>Les images sont trop lourdes et souvent les tailles ne correspondent pas aux versions mobiles.</t>
+  </si>
+  <si>
+    <t>Prévoir des images de tailles différentes pour mobiles et desktop et de format webp</t>
+  </si>
+  <si>
+    <t>Convertir les formats et créer des images pour les versions mobiles</t>
+  </si>
+  <si>
+    <t>Manque le code pour Google Analytics</t>
+  </si>
+  <si>
+    <t>Une vue statistique est importante pour connaitre les faiblesses du site et y apporter des correctifs</t>
+  </si>
+  <si>
+    <t>Toujours utiliser Google Analytics</t>
+  </si>
+  <si>
+    <t>Inclure le code de Google Analytics</t>
+  </si>
+  <si>
+    <t>√</t>
+  </si>
+  <si>
+    <t>Problèmes SEO et Accessibilité</t>
+  </si>
+  <si>
+    <t>Utiliser le plus possible les balises sémantiques</t>
+  </si>
+  <si>
+    <t>Faire les modifications</t>
+  </si>
+  <si>
+    <t>Cours</t>
+  </si>
+  <si>
+    <t>color.A11Y.com</t>
+  </si>
+  <si>
+    <t>Taille des fichiers CSS et JS</t>
+  </si>
+  <si>
+    <t>Les fichiers ne sont pas minifiés</t>
+  </si>
+  <si>
+    <t>Une fois le développement terminé, pensez à minifier les fichiers CSS et JS</t>
+  </si>
+  <si>
+    <t>PROBLÈMES</t>
+  </si>
+  <si>
+    <t>À proscrire, ne pas risquer un blacklistage</t>
+  </si>
+  <si>
+    <t>Modifier les couleurs et contrastes défectueux</t>
+  </si>
+  <si>
+    <t>Tester les couleurs et contrastes avant de les utiliser</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Les versions de </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>bootstrap.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> et</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> jquery.js</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sont trop anciennes, elles possèdent </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>9</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>failles</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> de sécurité à elles deux.</t>
+    </r>
+  </si>
+  <si>
+    <t>Balises sémantiques quasi inexistantes</t>
+  </si>
+  <si>
+    <t>Minifier les fichiers après modifications</t>
+  </si>
+  <si>
+    <t>Attention aux balises vides</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Balises vides et Class </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.icon-bar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> inexistantes</t>
+    </r>
+  </si>
+  <si>
+    <t>Permets une compatibilité avec les anciennes versions d’IE</t>
+  </si>
+  <si>
+    <t>Manque-le ; à la fin</t>
+  </si>
+  <si>
+    <t>mettre des couleurs différentes ou ne pas mettre en couleur les bordures</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>min-device-width</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> et </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>max-device-width</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sont déconseillés</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Mettre des icônes de lien, uniquement lorsque les liens sont disponibles. </t>
+  </si>
+  <si>
+    <t>Supprimer les icônes ou y mettre des liens</t>
+  </si>
+  <si>
+    <t>Optimiser les images</t>
+  </si>
+  <si>
+    <t>Gros problèmes d’accessibilité</t>
+  </si>
+  <si>
+    <t>Mettre à jour les versions, le code risque d’être à revoir</t>
+  </si>
+  <si>
+    <t>Tailles et format d’images non adaptés</t>
+  </si>
+  <si>
+    <t>La barre slash final n’a aucun effet</t>
+  </si>
+  <si>
+    <r>
+      <t>attribut </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>success-msg</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> non autorisé sur l’élément </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>form</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Déplacer le fichier et modifier le lien d’accès  href="</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>./css/style.css</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>"&gt;</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Supprimer les balises ne servant à rien et contrôler l’utilisation de la Class </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.icon-bar</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dans le reste du </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>CSS</t>
+    </r>
+  </si>
+  <si>
+    <t>Le label qui fonctionne avec le TextArea du dessous possède un ID au lieu d’un FOR, et le nom est commun au deux.</t>
+  </si>
+  <si>
+    <t>Mettre un FOR au Label pour l’associer au TextArea</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Erreur</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> : attribut </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">success-msg </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>et</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> fail-msg </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">non autorisé sur l’élément </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>form</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> à ce stade.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Il existe l’attribut </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>NOVALIDATE</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> qui empêche toute validation</t>
+    </r>
+  </si>
+  <si>
+    <t>n’est pas une valeur</t>
+  </si>
+  <si>
+    <r>
+      <t>La règle-arobase </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@-ms-viewport</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t> n’est pas reconnue</t>
+    </r>
+  </si>
+  <si>
+    <t>Dans le contexte, ceci n’est pas un problème</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>none</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> était utilisé en CSS 2.1, alors qu’en CSS 3 c’est remplacé par </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>never</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Propriété erronée : padding-left </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>constant</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(safe-area-inset-left) n’est pas une valeur de padding-left : </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>constant</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(safe-area-inset-left)</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>constant</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> n’est pas reconnu</t>
+    </r>
+  </si>
+  <si>
+    <t>Titre et Texte ci-dessus ne sont pas centrés malgré l’utilisation de la class text-center de bootstrap.css</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">J’ai créé et ajouté la class </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>center</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> aux balises </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>H1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> et </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FF00B050"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>P</t>
+    </r>
+  </si>
+  <si>
+    <t>Vérifier le bon fonctionnement des class venant d’autres fichiers css</t>
+  </si>
+  <si>
+    <t>Ils ne servent à rien en l’état actuel</t>
+  </si>
+  <si>
+    <t>Le contraste n’est pas bon sur le texte du Footer</t>
+  </si>
+  <si>
+    <t>Le poids et les formats d’images sont trop lourds pour la plupart.</t>
+  </si>
+  <si>
+    <r>
       <t>Manque la balise</t>
     </r>
     <r>
@@ -1204,7 +1890,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t>&lt;description&gt;</t>
+      <t>&lt; meta description&gt;</t>
     </r>
     <r>
       <rPr>
@@ -1215,692 +1901,6 @@
       </rPr>
       <t xml:space="preserve"> est vide</t>
     </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Des balises </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>&lt;meta&gt;</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> importantes sont absentes</t>
-    </r>
-  </si>
-  <si>
-    <t>Ne pas oublier ces balises</t>
-  </si>
-  <si>
-    <t>Ajouter ces balises</t>
-  </si>
-  <si>
-    <t>Les images sont trop lourdes et souvent les tailles ne correspondent pas aux versions mobiles.</t>
-  </si>
-  <si>
-    <t>Prévoir des images de tailles différentes pour mobiles et desktop et de format webp</t>
-  </si>
-  <si>
-    <t>Convertir les formats et créer des images pour les versions mobiles</t>
-  </si>
-  <si>
-    <t>Manque le code pour Google Analytics</t>
-  </si>
-  <si>
-    <t>Une vue statistique est importante pour connaitre les faiblesses du site et y apporter des correctifs</t>
-  </si>
-  <si>
-    <t>Toujours utiliser Google Analytics</t>
-  </si>
-  <si>
-    <t>Inclure le code de Google Analytics</t>
-  </si>
-  <si>
-    <t>√</t>
-  </si>
-  <si>
-    <t>Problèmes SEO et Accessibilité</t>
-  </si>
-  <si>
-    <t>Utiliser le plus possible les balises sémantiques</t>
-  </si>
-  <si>
-    <t>Faire les modifications</t>
-  </si>
-  <si>
-    <t>Cours</t>
-  </si>
-  <si>
-    <t>color.A11Y.com</t>
-  </si>
-  <si>
-    <t>Taille des fichiers CSS et JS</t>
-  </si>
-  <si>
-    <t>Les fichiers ne sont pas minifiés</t>
-  </si>
-  <si>
-    <t>Une fois le développement terminé, pensez à minifier les fichiers CSS et JS</t>
-  </si>
-  <si>
-    <t>PROBLÈMES</t>
-  </si>
-  <si>
-    <t>À proscrire, ne pas risquer un blacklistage</t>
-  </si>
-  <si>
-    <t>Modifier les couleurs et contrastes défectueux</t>
-  </si>
-  <si>
-    <t>Tester les couleurs et contrastes avant de les utiliser</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Les versions de </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>bootstrap.js</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> et</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> jquery.js</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> sont trop anciennes, elles possèdent </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>9</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>failles</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> de sécurité à elles deux.</t>
-    </r>
-  </si>
-  <si>
-    <t>Balises sémantiques quasi inexistantes</t>
-  </si>
-  <si>
-    <t>Minifier les fichiers après modifications</t>
-  </si>
-  <si>
-    <t>Attention aux balises vides</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Balises vides et Class </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.icon-bar</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> inexistantes</t>
-    </r>
-  </si>
-  <si>
-    <t>Permets une compatibilité avec les anciennes versions d’IE</t>
-  </si>
-  <si>
-    <t>Manque-le ; à la fin</t>
-  </si>
-  <si>
-    <t>mettre des couleurs différentes ou ne pas mettre en couleur les bordures</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>min-device-width</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> et </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>max-device-width</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> sont déconseillés</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Mettre des icônes de lien, uniquement lorsque les liens sont disponibles. </t>
-  </si>
-  <si>
-    <t>Supprimer les icônes ou y mettre des liens</t>
-  </si>
-  <si>
-    <t>Optimiser les images</t>
-  </si>
-  <si>
-    <t>Gros problèmes d’accessibilité</t>
-  </si>
-  <si>
-    <t>Mettre à jour les versions, le code risque d’être à revoir</t>
-  </si>
-  <si>
-    <t>Tailles et format d’images non adaptés</t>
-  </si>
-  <si>
-    <t>La barre slash final n’a aucun effet</t>
-  </si>
-  <si>
-    <r>
-      <t>attribut </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>success-msg</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> non autorisé sur l’élément </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>form</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Déplacer le fichier et modifier le lien d’accès  href="</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>./css/style.css</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"&gt;</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Supprimer les balises ne servant à rien et contrôler l’utilisation de la Class </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>.icon-bar</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> dans le reste du </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>CSS</t>
-    </r>
-  </si>
-  <si>
-    <t>Le label qui fonctionne avec le TextArea du dessous possède un ID au lieu d’un FOR, et le nom est commun au deux.</t>
-  </si>
-  <si>
-    <t>Mettre un FOR au Label pour l’associer au TextArea</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Erreur</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> : attribut </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">success-msg </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>et</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> fail-msg </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">non autorisé sur l’élément </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>form</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> à ce stade.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Il existe l’attribut </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>NOVALIDATE</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> qui empêche toute validation</t>
-    </r>
-  </si>
-  <si>
-    <t>n’est pas une valeur</t>
-  </si>
-  <si>
-    <r>
-      <t>La règle-arobase </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>@-ms-viewport</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t> n’est pas reconnue</t>
-    </r>
-  </si>
-  <si>
-    <t>Dans le contexte, ceci n’est pas un problème</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>none</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> était utilisé en CSS 2.1, alors qu’en CSS 3 c’est remplacé par </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>never</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Propriété erronée : padding-left </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>constant</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(safe-area-inset-left) n’est pas une valeur de padding-left : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>constant</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>(safe-area-inset-left)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>constant</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> n’est pas reconnu</t>
-    </r>
-  </si>
-  <si>
-    <t>Titre et Texte ci-dessus ne sont pas centrés malgré l’utilisation de la class text-center de bootstrap.css</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">J’ai créé et ajouté la class </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>center</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> aux balises </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>H1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> et </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color rgb="FF00B050"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>P</t>
-    </r>
-  </si>
-  <si>
-    <t>Vérifier le bon fonctionnement des class venant d’autres fichiers css</t>
-  </si>
-  <si>
-    <t>Ils ne servent à rien en l’état actuel</t>
-  </si>
-  <si>
-    <t>Le contraste n’est pas bon sur le texte du Footer</t>
-  </si>
-  <si>
-    <t>Le poids et les formats d’images sont trop lourds pour la plupart.</t>
   </si>
 </sst>
 </file>
@@ -2177,6 +2177,18 @@
     <xf numFmtId="2" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2190,18 +2202,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2429,7 +2429,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B19" sqref="B19"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.27734375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.4"/>
@@ -2487,16 +2487,16 @@
       <c r="Z1" s="6"/>
     </row>
     <row r="2" spans="1:26" s="7" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="23" t="s">
-        <v>132</v>
-      </c>
-      <c r="B2" s="24"/>
-      <c r="C2" s="24"/>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24"/>
-      <c r="F2" s="24"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="28"/>
+      <c r="A2" s="27" t="s">
+        <v>131</v>
+      </c>
+      <c r="B2" s="28"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="23"/>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
       <c r="K2" s="6"/>
@@ -2533,13 +2533,13 @@
         <v>102</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G3" s="21">
         <v>22</v>
       </c>
-      <c r="H3" s="29" t="s">
-        <v>123</v>
+      <c r="H3" s="24" t="s">
+        <v>122</v>
       </c>
       <c r="I3" s="18"/>
       <c r="J3" s="18"/>
@@ -2561,7 +2561,7 @@
       <c r="Z3" s="18"/>
     </row>
     <row r="4" spans="1:26" s="19" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="25" t="s">
         <v>92</v>
       </c>
       <c r="B4" s="21" t="s">
@@ -2571,17 +2571,17 @@
         <v>106</v>
       </c>
       <c r="D4" s="21" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E4" s="21" t="s">
         <v>107</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G4" s="21"/>
-      <c r="H4" s="29" t="s">
-        <v>123</v>
+      <c r="H4" s="24" t="s">
+        <v>122</v>
       </c>
       <c r="I4" s="18"/>
       <c r="J4" s="18"/>
@@ -2607,23 +2607,23 @@
         <v>92</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C5" s="21" t="s">
         <v>108</v>
       </c>
       <c r="D5" s="21" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E5" s="21" t="s">
-        <v>134</v>
-      </c>
-      <c r="F5" s="31" t="s">
-        <v>128</v>
+        <v>133</v>
+      </c>
+      <c r="F5" s="26" t="s">
+        <v>127</v>
       </c>
       <c r="G5" s="21"/>
-      <c r="H5" s="29" t="s">
-        <v>123</v>
+      <c r="H5" s="24" t="s">
+        <v>122</v>
       </c>
       <c r="I5" s="18"/>
       <c r="J5" s="18"/>
@@ -2645,27 +2645,27 @@
       <c r="Z5" s="18"/>
     </row>
     <row r="6" spans="1:26" s="19" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="25" t="s">
         <v>92</v>
       </c>
       <c r="B6" s="21" t="s">
         <v>109</v>
       </c>
       <c r="C6" s="21" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D6" s="21" t="s">
         <v>110</v>
       </c>
       <c r="E6" s="21" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F6" s="21" t="s">
         <v>111</v>
       </c>
       <c r="G6" s="21"/>
-      <c r="H6" s="29" t="s">
-        <v>123</v>
+      <c r="H6" s="24" t="s">
+        <v>122</v>
       </c>
       <c r="I6" s="18"/>
       <c r="J6" s="18"/>
@@ -2691,23 +2691,23 @@
         <v>92</v>
       </c>
       <c r="B7" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>170</v>
+      </c>
+      <c r="D7" s="21" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="21" t="s">
-        <v>112</v>
-      </c>
-      <c r="D7" s="21" t="s">
+      <c r="E7" s="21" t="s">
         <v>114</v>
       </c>
-      <c r="E7" s="21" t="s">
-        <v>115</v>
-      </c>
       <c r="F7" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G7" s="21"/>
-      <c r="H7" s="29" t="s">
-        <v>123</v>
+      <c r="H7" s="24" t="s">
+        <v>122</v>
       </c>
       <c r="I7" s="18"/>
       <c r="J7" s="18"/>
@@ -2729,27 +2729,27 @@
       <c r="Z7" s="18"/>
     </row>
     <row r="8" spans="1:26" s="19" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="25" t="s">
         <v>92</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C8" s="21" t="s">
+        <v>115</v>
+      </c>
+      <c r="D8" s="21" t="s">
         <v>116</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="E8" s="21" t="s">
         <v>117</v>
-      </c>
-      <c r="E8" s="21" t="s">
-        <v>118</v>
       </c>
       <c r="F8" s="21" t="s">
         <v>87</v>
       </c>
       <c r="G8" s="21"/>
-      <c r="H8" s="29" t="s">
-        <v>123</v>
+      <c r="H8" s="24" t="s">
+        <v>122</v>
       </c>
       <c r="I8" s="18"/>
       <c r="J8" s="18"/>
@@ -2775,23 +2775,23 @@
         <v>39</v>
       </c>
       <c r="B9" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="C9" s="21" t="s">
         <v>119</v>
       </c>
-      <c r="C9" s="21" t="s">
+      <c r="D9" s="21" t="s">
         <v>120</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="E9" s="21" t="s">
         <v>121</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="F9" s="21" t="s">
+        <v>126</v>
+      </c>
+      <c r="G9" s="21"/>
+      <c r="H9" s="24" t="s">
         <v>122</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>127</v>
-      </c>
-      <c r="G9" s="21"/>
-      <c r="H9" s="29" t="s">
-        <v>123</v>
       </c>
       <c r="I9" s="18"/>
       <c r="J9" s="18"/>
@@ -2813,27 +2813,27 @@
       <c r="Z9" s="18"/>
     </row>
     <row r="10" spans="1:26" s="19" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="30" t="s">
+      <c r="A10" s="25" t="s">
         <v>92</v>
       </c>
       <c r="B10" s="21" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="21" t="s">
+        <v>136</v>
+      </c>
+      <c r="D10" s="21" t="s">
         <v>124</v>
       </c>
-      <c r="C10" s="21" t="s">
-        <v>137</v>
-      </c>
-      <c r="D10" s="21" t="s">
+      <c r="E10" s="21" t="s">
         <v>125</v>
       </c>
-      <c r="E10" s="21" t="s">
+      <c r="F10" s="21" t="s">
         <v>126</v>
       </c>
-      <c r="F10" s="21" t="s">
-        <v>127</v>
-      </c>
       <c r="G10" s="21"/>
-      <c r="H10" s="29" t="s">
-        <v>123</v>
+      <c r="H10" s="24" t="s">
+        <v>122</v>
       </c>
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
@@ -2859,23 +2859,23 @@
         <v>92</v>
       </c>
       <c r="B11" s="21" t="s">
+        <v>128</v>
+      </c>
+      <c r="C11" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="C11" s="21" t="s">
+      <c r="D11" s="21" t="s">
         <v>130</v>
       </c>
-      <c r="D11" s="21" t="s">
-        <v>131</v>
-      </c>
       <c r="E11" s="21" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G11" s="21"/>
-      <c r="H11" s="29" t="s">
-        <v>123</v>
+      <c r="H11" s="24" t="s">
+        <v>122</v>
       </c>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
@@ -2897,16 +2897,16 @@
       <c r="Z11" s="18"/>
     </row>
     <row r="12" spans="1:26" s="7" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="24"/>
-      <c r="C12" s="24"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
-      <c r="F12" s="24"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="29"/>
+      <c r="H12" s="23"/>
       <c r="I12" s="6"/>
       <c r="J12" s="6"/>
       <c r="K12" s="6"/>
@@ -2955,7 +2955,7 @@
         <v>8</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>90</v>
@@ -2975,7 +2975,7 @@
         <v>40</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>10</v>
@@ -3005,7 +3005,7 @@
         <v>95</v>
       </c>
       <c r="E16" s="13" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="F16" s="13"/>
       <c r="G16" s="13">
@@ -3023,7 +3023,7 @@
         <v>49</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E17" s="3" t="s">
         <v>50</v>
@@ -3041,13 +3041,13 @@
         <v>57</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>58</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="13">
@@ -3062,10 +3062,10 @@
         <v>59</v>
       </c>
       <c r="C19" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="D19" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="D19" s="3" t="s">
-        <v>156</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>62</v>
@@ -3082,10 +3082,10 @@
         <v>40</v>
       </c>
       <c r="B20" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="C20" s="13" t="s">
         <v>157</v>
-      </c>
-      <c r="C20" s="13" t="s">
-        <v>158</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>60</v>
@@ -3101,15 +3101,15 @@
       </c>
     </row>
     <row r="21" spans="1:7" s="7" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="23" t="s">
+      <c r="A21" s="27" t="s">
         <v>41</v>
       </c>
-      <c r="B21" s="26"/>
-      <c r="C21" s="26"/>
-      <c r="D21" s="26"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="26"/>
-      <c r="G21" s="27"/>
+      <c r="B21" s="30"/>
+      <c r="C21" s="30"/>
+      <c r="D21" s="30"/>
+      <c r="E21" s="30"/>
+      <c r="F21" s="30"/>
+      <c r="G21" s="31"/>
     </row>
     <row r="22" spans="1:7" s="7" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A22" s="4" t="s">
@@ -3119,10 +3119,10 @@
         <v>43</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>96</v>
@@ -3140,7 +3140,7 @@
         <v>12</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="13" t="s">
@@ -3183,7 +3183,7 @@
         <v>15</v>
       </c>
       <c r="D25" s="13" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E25" s="13" t="s">
         <v>26</v>
@@ -3204,7 +3204,7 @@
         <v>17</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>16</v>
@@ -3219,7 +3219,7 @@
         <v>42</v>
       </c>
       <c r="B27" s="13" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C27" s="13" t="s">
         <v>19</v>
@@ -3268,7 +3268,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="13" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="D29" s="13"/>
       <c r="E29" s="13"/>
@@ -3308,7 +3308,7 @@
         <v>45</v>
       </c>
       <c r="C31" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="D31" s="13" t="s">
         <v>46</v>
@@ -3328,7 +3328,7 @@
         <v>52</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>53</v>
@@ -3349,10 +3349,10 @@
         <v>52</v>
       </c>
       <c r="B33" s="13" t="s">
+        <v>162</v>
+      </c>
+      <c r="C33" s="13" t="s">
         <v>163</v>
-      </c>
-      <c r="C33" s="13" t="s">
-        <v>164</v>
       </c>
       <c r="D33" s="13" t="s">
         <v>63</v>
@@ -3368,15 +3368,15 @@
       </c>
     </row>
     <row r="34" spans="1:8" s="7" customFormat="1" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="23" t="s">
+      <c r="A34" s="27" t="s">
         <v>71</v>
       </c>
-      <c r="B34" s="26"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
-      <c r="G34" s="27"/>
+      <c r="B34" s="30"/>
+      <c r="C34" s="30"/>
+      <c r="D34" s="30"/>
+      <c r="E34" s="30"/>
+      <c r="F34" s="30"/>
+      <c r="G34" s="31"/>
     </row>
     <row r="35" spans="1:8" s="7" customFormat="1" ht="48" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A35" s="9" t="s">
@@ -3395,7 +3395,7 @@
         <v>76</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G35" s="3" t="s">
         <v>75</v>
@@ -3406,13 +3406,13 @@
         <v>40</v>
       </c>
       <c r="B36" s="13" t="s">
+        <v>164</v>
+      </c>
+      <c r="C36" s="13" t="s">
         <v>165</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="D36" s="13" t="s">
         <v>166</v>
-      </c>
-      <c r="D36" s="13" t="s">
-        <v>167</v>
       </c>
       <c r="E36" s="13" t="s">
         <v>77</v>
@@ -3430,13 +3430,13 @@
         <v>78</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D37" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>145</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>146</v>
       </c>
       <c r="F37" s="3" t="s">
         <v>79</v>
@@ -3445,7 +3445,7 @@
         <v>97</v>
       </c>
       <c r="H37" s="22" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:8" s="14" customFormat="1" ht="32" customHeight="1" x14ac:dyDescent="0.4">
@@ -3453,7 +3453,7 @@
         <v>39</v>
       </c>
       <c r="B38" s="13" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="C38" s="13" t="s">
         <v>80</v>
@@ -3495,13 +3495,13 @@
         <v>89</v>
       </c>
       <c r="B40" s="13" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="C40" s="13" t="s">
         <v>86</v>
       </c>
       <c r="D40" s="13" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E40" s="13" t="s">
         <v>99</v>

</xml_diff>